<commit_message>
kit de montage freinage
</commit_message>
<xml_diff>
--- a/Kit_montage_antiroll bar_a terminer.xlsx
+++ b/Kit_montage_antiroll bar_a terminer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\EPSA_git\STUF2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C262E0E-9057-4CDC-B941-AEE45722B85A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0990D9F2-4F59-4DC3-A55F-CA59167609E3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="6114" windowHeight="8154" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -186,12 +186,6 @@
     </r>
   </si>
   <si>
-    <t>Carrosserie</t>
-  </si>
-  <si>
-    <t>Josselin KIEFEL</t>
-  </si>
-  <si>
     <t>Barre avant</t>
   </si>
   <si>
@@ -250,6 +244,12 @@
   </si>
   <si>
     <t xml:space="preserve">Ecrous M6 </t>
+  </si>
+  <si>
+    <t>Barre anti-roulis</t>
+  </si>
+  <si>
+    <t>Erwan de Longcamp</t>
   </si>
 </sst>
 </file>
@@ -533,7 +533,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -546,16 +554,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -873,7 +873,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -893,12 +893,12 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
       <c r="F1" s="1"/>
       <c r="G1" s="7" t="s">
         <v>4</v>
@@ -914,35 +914,35 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.85">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
       <c r="E3" s="20" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="3" customFormat="1" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="1">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="28"/>
       <c r="E5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:9" s="3" customFormat="1" ht="19.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.95">
       <c r="A6" s="22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -965,7 +965,7 @@
     </row>
     <row r="7" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A7" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -988,7 +988,7 @@
     </row>
     <row r="8" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A8" s="21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="9" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A9" s="21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="10" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A10" s="21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="11" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A11" s="21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="12" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A12" s="21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1103,7 +1103,7 @@
     </row>
     <row r="13" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A13" s="21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="14" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A14" s="21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="15" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A15" s="21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="16" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A16" s="21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="17" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A17" s="21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1218,7 +1218,7 @@
     </row>
     <row r="18" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A18" s="21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1241,7 +1241,7 @@
     </row>
     <row r="19" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A19" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="20" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A20" s="21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="21" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A21" s="21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1392,25 +1392,25 @@
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:9" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="1">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="26"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="28"/>
       <c r="E27" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9" ht="19.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.95">
       <c r="A28" s="21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
@@ -1421,17 +1421,17 @@
       <c r="F28" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="H28" s="29"/>
+      <c r="G28" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" s="32"/>
       <c r="I28" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A29" s="23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -1442,17 +1442,17 @@
       <c r="F29" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="H29" s="24"/>
+      <c r="G29" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" s="31"/>
       <c r="I29" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A30" s="23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -1463,17 +1463,17 @@
       <c r="F30" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="H30" s="24"/>
+      <c r="G30" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H30" s="31"/>
       <c r="I30" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A31" s="23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -1484,17 +1484,17 @@
       <c r="F31" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="H31" s="24"/>
+      <c r="G31" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="31"/>
       <c r="I31" s="13" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A32" s="23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -1505,10 +1505,10 @@
       <c r="F32" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="H32" s="24"/>
+      <c r="G32" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="31"/>
       <c r="I32" s="13" t="s">
         <v>6</v>
       </c>
@@ -1522,10 +1522,10 @@
       <c r="F33" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G33" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="H33" s="24"/>
+      <c r="G33" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" s="31"/>
       <c r="I33" s="13" t="s">
         <v>6</v>
       </c>
@@ -1553,11 +1553,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="G31:H31"/>
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="G33:H33"/>
     <mergeCell ref="A27:D27"/>
@@ -1565,6 +1560,11 @@
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G30:H30"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="G31:H31"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>